<commit_message>
Ongoing Chapter 3 Writing
</commit_message>
<xml_diff>
--- a/RRLs/keyword_Volume Measurement using Point cloud.xlsx
+++ b/RRLs/keyword_Volume Measurement using Point cloud.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gmsuiiteduph-my.sharepoint.com/personal/jaafar_omar0701_g_msuiit_edu_ph/Documents/MSci Documents/Master's Thesis/For final defense/RRL/Sorted/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gmsuiiteduph-my.sharepoint.com/personal/jaafar_omar0701_g_msuiit_edu_ph/Documents/MSci Documents/LaTeX programs/Manuscript_Omar/RRLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1E03E1D0-9B6A-457D-BF53-7456356BA1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{1E03E1D0-9B6A-457D-BF53-7456356BA1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F742766-C018-4271-9CEF-387C0A9C08D0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_google-scholar-scraper_" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3175,7 +3188,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3306,6 +3319,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3608,7 +3629,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -3651,14 +3672,16 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -3692,6 +3715,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -4034,12 +4058,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="P109" sqref="P109"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="48.42578125" customWidth="1"/>
     <col min="15" max="15" width="52" style="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" customWidth="1"/>
     <col min="17" max="17" width="47.28515625" style="1" customWidth="1"/>
@@ -4138,7 +4164,7 @@
       <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L2" t="s">
@@ -4200,7 +4226,7 @@
       <c r="I3" t="s">
         <v>37</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L3" t="s">
@@ -10311,6 +10337,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{02109F2A-47E8-4D49-93B6-8DCADE615C66}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{015F7706-4A27-4C14-92DC-3C6C6F645F6D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>